<commit_message>
Coding target population in Round one
</commit_message>
<xml_diff>
--- a/2_Raw_Data/2_1_TPS/BTS_key_words_code_final.xlsx
+++ b/2_Raw_Data/2_1_TPS/BTS_key_words_code_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuwe\Desktop\大团队科学样本代表性\BTS_Sample_Stage1_RR\BTS_Sample_Stage1_RR\2_Raw_Data\2_1_TPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F35194-5EF1-4D4C-A1A8-A823B98DD969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA72CA4C-DF13-46D2-9D3A-D36572452C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="822" windowWidth="19110" windowHeight="9006" xr2:uid="{D65725F8-0F32-408D-940F-7254C93BA44D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="11472" xr2:uid="{D65725F8-0F32-408D-940F-7254C93BA44D}"/>
   </bookViews>
   <sheets>
     <sheet name="001BTS_all_wcx_20251031" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
   <si>
     <t>ID</t>
   </si>
@@ -479,15 +479,6 @@
   </si>
   <si>
     <t>The general fault in our fault lines</t>
-  </si>
-  <si>
-    <t>Sirota, Miroslav; 艩rol, Jakub; Lisi, Matteo; Juanchich, Marie; Wolfe, Kelly; Buchanan, Erin M.</t>
-  </si>
-  <si>
-    <t>22Mapping and Increasing Error Correction Behaviour in a Culturally Diverse Sample</t>
-  </si>
-  <si>
-    <t>Error Correction, Intuitive Reasoning, Cultural Diversity, Feedback, Justification</t>
   </si>
   <si>
     <t>Sorokowski, Piotr; Kowal, Marta; Sternberg, Robert J.; Aavik, Toivo; Akello, Grace; Alhabahba, Mohammad Madallh; Alm, Charlotte; Amjad, Naumana; Anjum, Afifa; Asao, Kelly; Atama, Chiemezie S.; Atamt眉rk Duyar, Derya; Ayebare, Richard; Conroy-Beam, Daniel; Bendixen, Mons; Bensafia, Aicha; Bizumic, Boris; Boussena, Mahmoud; Buss, David M.; Butovskaya, Marina; Can, Seda; Carrier, Antonin; Cetinkaya, Hakan; Croy, Ilona; Cueto, Rosa Mar铆a; Czub, Marcin; Dronova, Daria; Dural, Seda; Duyar, Izzet; Ertugrul, Berna; Espinosa, Agust铆n; Estevan, Ignacio; Esteves, Carla Sofia; Frackowiak, Tomasz; Gardu帽o, Jorge Contreras; Gonz谩lez, Karina Ugalde; Guemaz, Farida; Halamov谩, M谩ria; Herak, Iskra; Horvat, Marina; Hromatko, Ivana; Hui, Chin-Ming; Jaafar, Jas Laile; Jiang, Feng; Kafetsios, Konstantinos; Kav膷i膷, Tina; Kennair, Leif Edward Ottesen; Kervyn, Nicolas; Ha, Truong Thi Khanh; Khilji, Imran Ahmed; K枚bis, Nils C.; Kostic, Aleksandra; Lan, Hoang Moc; L谩ng, Andr谩s; Lennard, Georgina R.; Le贸n, Ernesto; Lindholm, Torun; Linh, Trinh Thi; Lopez, Giulia; Van Luot, Nguyen; Mailhos, Alvaro; Manesi, Zoi; Martinez, Rocio; McKerchar, Sarah L.; Mesk贸, Norbert; Peji膷i膰, Marija; Misra, Girishwar; Monaghan, Conal; Mora, Emanuel C.; Moya-Gar贸fano, Alba; Musil, Bojan; Natividade, Jean Carlos; Nizharadze, George; Oberzaucher, Elisabeth; Oleszkiewicz, Anna; Omar-Fauzee, Mohd Sofian; Onyishi, Ike E.; 脰zener, Baris; Pagani, Ariela Francesca; Pakalniskiene, Vilmante; Parise, Miriam; Pazhoohi, Farid; Pisanski, Annette; Pisanski, Katarzyna; Ponciano, Edna; Popa, Camelia; Prokop, Pavol; Rizwan, Muhammad; Sainz, Mario; Salki膷evi膰, Svjetlana; Sargautyte, Ruta; Sarm谩ny-Schuller, Ivan; Schmehl, Susanne; Shahid, Anam; Sharad, Shivantika; Siddiqui, Razi Sultan; Simonetti, Franco; Tadinac, Meri; Vauclair, Christin-Melanie; Vega, Luis Diego; Walter, Kathryn V.; Widarini, Dwi Ajeng; Yoo, Gyesook; Za钮kov谩, Marta; Zupan膷i膷, Maja; Sorokowska, Agnieszka</t>
@@ -1692,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00A682E-359B-40D2-AA62-2EFDEBBAE5C0}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1727,7 +1718,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1758,7 +1749,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
@@ -1772,7 +1763,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -1800,7 +1791,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
@@ -1811,10 +1802,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -1828,7 +1819,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -1856,7 +1847,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -1870,7 +1861,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
@@ -1884,7 +1875,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
@@ -1898,7 +1889,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -1912,7 +1903,7 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
@@ -1990,7 +1981,7 @@
         <v>99000020</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
         <v>49</v>
@@ -2175,10 +2166,10 @@
         <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
@@ -2192,7 +2183,7 @@
         <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -2220,7 +2211,7 @@
         <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -2276,7 +2267,7 @@
         <v>105</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
@@ -2413,10 +2404,10 @@
         <v>133</v>
       </c>
       <c r="C51" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.5">
@@ -2500,7 +2491,7 @@
         <v>150</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.5">
@@ -2514,7 +2505,7 @@
         <v>152</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.5">
@@ -2527,8 +2518,8 @@
       <c r="C59" t="s">
         <v>154</v>
       </c>
-      <c r="D59" t="s">
-        <v>155</v>
+      <c r="D59" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.5">
@@ -2536,13 +2527,13 @@
         <v>99000059</v>
       </c>
       <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" t="s">
         <v>156</v>
       </c>
-      <c r="C60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>208</v>
+      <c r="D60" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.5">
@@ -2550,31 +2541,31 @@
         <v>99000060</v>
       </c>
       <c r="B61" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" t="s">
         <v>158</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>159</v>
       </c>
-      <c r="D61" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="62" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>99000061</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="2">
+      <c r="A63">
         <v>99000062</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2588,35 +2579,35 @@
       </c>
     </row>
     <row r="64" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="2">
+      <c r="A64">
         <v>99000063</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A65">
+        <v>99000064</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="2">
-        <v>99000064</v>
-      </c>
-      <c r="B65" s="2" t="s">
+      <c r="D65" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="3">
+      <c r="A66">
         <v>99000065</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -2629,17 +2620,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A67">
         <v>99000066</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" t="s">
         <v>173</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" t="s">
         <v>174</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2653,8 +2644,8 @@
       <c r="C68" t="s">
         <v>177</v>
       </c>
-      <c r="D68" t="s">
-        <v>178</v>
+      <c r="D68" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.5">
@@ -2662,13 +2653,13 @@
         <v>99000068</v>
       </c>
       <c r="B69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" t="s">
         <v>179</v>
       </c>
-      <c r="C69" t="s">
-        <v>180</v>
-      </c>
       <c r="D69" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.5">
@@ -2676,31 +2667,31 @@
         <v>99000069</v>
       </c>
       <c r="B70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
         <v>181</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>182</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="71" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>99000070</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A72" s="2">
+      <c r="A72">
         <v>99000071</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -2714,7 +2705,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A73" s="2">
+      <c r="A73">
         <v>99000072</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -2724,21 +2715,7 @@
         <v>190</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A74" s="2">
-        <v>99000073</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>